<commit_message>
update on null for berikutnya
</commit_message>
<xml_diff>
--- a/temp/excelTestCheckup.xlsx
+++ b/temp/excelTestCheckup.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="47">
   <si>
     <t>posyandu</t>
   </si>
@@ -50,19 +50,109 @@
     <t>POSYANDU X</t>
   </si>
   <si>
+    <t>235236</t>
+  </si>
+  <si>
+    <t>Kucing</t>
+  </si>
+  <si>
+    <t>Rumah awan</t>
+  </si>
+  <si>
+    <t>awan</t>
+  </si>
+  <si>
+    <t>2023-02-04</t>
+  </si>
+  <si>
+    <t>42424251</t>
+  </si>
+  <si>
+    <t>Balita new dari sendiri 2</t>
+  </si>
+  <si>
+    <t>Rumah ADMIn</t>
+  </si>
+  <si>
+    <t>admi</t>
+  </si>
+  <si>
+    <t>2023-03-08</t>
+  </si>
+  <si>
+    <t>Balita new dari sendiri 23</t>
+  </si>
+  <si>
+    <t>42424250</t>
+  </si>
+  <si>
+    <t>Balita new dari sendiri 20</t>
+  </si>
+  <si>
+    <t>2023-03-20</t>
+  </si>
+  <si>
     <t>777777</t>
   </si>
   <si>
     <t>Balita new dari sendiri 14</t>
   </si>
   <si>
-    <t>Rumah ADMIn</t>
-  </si>
-  <si>
-    <t>admi</t>
-  </si>
-  <si>
     <t>2023-04-20</t>
+  </si>
+  <si>
+    <t>231</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>Rumah Rafli</t>
+  </si>
+  <si>
+    <t>BUKAN RAFLI SUMPA</t>
+  </si>
+  <si>
+    <t>2023-02-24</t>
+  </si>
+  <si>
+    <t>12451325235</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>Balita User 1</t>
+  </si>
+  <si>
+    <t>Rumah User 2</t>
+  </si>
+  <si>
+    <t>User 2</t>
+  </si>
+  <si>
+    <t>2023-03-26</t>
+  </si>
+  <si>
+    <t>912841</t>
+  </si>
+  <si>
+    <t>Tuki</t>
+  </si>
+  <si>
+    <t>Rumah lain</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>2023-03-27</t>
+  </si>
+  <si>
+    <t>234634</t>
+  </si>
+  <si>
+    <t>Bambang</t>
   </si>
 </sst>
 </file>
@@ -107,7 +197,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -116,14 +206,14 @@
     <col min="1" max="1" width="12.8125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="7.70703125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="23.65625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="8.70703125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="7.3359375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="13.3046875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="12.7421875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="9.99609375" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.15234375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="14.17578125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="20.1484375" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="15.015625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="12.7421875" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="6.01171875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="12.7421875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -166,7 +256,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="n" s="0">
-        <v>10.0</v>
+        <v>4.0</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>13</v>
@@ -175,10 +265,10 @@
         <v>12</v>
       </c>
       <c r="E2" t="n">
-        <v>20.0</v>
+        <v>5.0</v>
       </c>
       <c r="F2" t="n">
-        <v>10.0</v>
+        <v>2.0</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
@@ -190,10 +280,325 @@
         <v>16</v>
       </c>
       <c r="J2" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1.2999999523162842</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B3" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>11.300000190734863</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B4" t="n" s="0">
+        <v>8.0</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B5" t="n" s="0">
+        <v>9.0</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" t="n">
+        <v>5.099999904632568</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1.100000023841858</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B6" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" t="n">
         <v>7.099999904632568</v>
       </c>
-      <c r="K2" t="n">
+      <c r="K6" t="n">
         <v>21.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B7" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1.7000000476837158</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B8" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B9" t="n" s="0">
+        <v>11.0</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2.700000047683716</v>
+      </c>
+      <c r="F9" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="K9" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B10" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B11" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" t="n">
+        <v>213.0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added for reporting 30 days data and healty data
</commit_message>
<xml_diff>
--- a/temp/excelTestCheckup.xlsx
+++ b/temp/excelTestCheckup.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
   <si>
     <t>posyandu</t>
   </si>
@@ -119,6 +119,36 @@
     <t>12451325235</t>
   </si>
   <si>
+    <t>912841</t>
+  </si>
+  <si>
+    <t>Tuki</t>
+  </si>
+  <si>
+    <t>Rumah lain</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>2023-03-27</t>
+  </si>
+  <si>
+    <t>234634</t>
+  </si>
+  <si>
+    <t>Bambang</t>
+  </si>
+  <si>
+    <t>12309162309</t>
+  </si>
+  <si>
+    <t>Balita baru tanggal ini</t>
+  </si>
+  <si>
+    <t>2023-05-09</t>
+  </si>
+  <si>
     <t>21</t>
   </si>
   <si>
@@ -134,25 +164,13 @@
     <t>2023-03-26</t>
   </si>
   <si>
-    <t>912841</t>
-  </si>
-  <si>
-    <t>Tuki</t>
-  </si>
-  <si>
-    <t>Rumah lain</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>2023-03-27</t>
-  </si>
-  <si>
-    <t>234634</t>
-  </si>
-  <si>
-    <t>Bambang</t>
+    <t>31</t>
+  </si>
+  <si>
+    <t>Freya</t>
+  </si>
+  <si>
+    <t>2023-04-27</t>
   </si>
 </sst>
 </file>
@@ -197,7 +215,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -501,7 +519,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="n" s="0">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="C9" t="s" s="0">
         <v>36</v>
@@ -510,10 +528,10 @@
         <v>35</v>
       </c>
       <c r="E9" t="n">
-        <v>2.700000047683716</v>
+        <v>23.0</v>
       </c>
       <c r="F9" t="n">
-        <v>47.0</v>
+        <v>10.0</v>
       </c>
       <c r="G9" t="s">
         <v>37</v>
@@ -525,10 +543,10 @@
         <v>39</v>
       </c>
       <c r="J9" t="n">
-        <v>5.5</v>
+        <v>8.0</v>
       </c>
       <c r="K9" t="n">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="10">
@@ -536,7 +554,7 @@
         <v>11</v>
       </c>
       <c r="B10" t="n" s="0">
-        <v>12.0</v>
+        <v>2.0</v>
       </c>
       <c r="C10" t="s" s="0">
         <v>41</v>
@@ -545,25 +563,25 @@
         <v>40</v>
       </c>
       <c r="E10" t="n">
-        <v>23.0</v>
+        <v>5.0</v>
       </c>
       <c r="F10" t="n">
-        <v>10.0</v>
+        <v>2.0</v>
       </c>
       <c r="G10" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="H10" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="I10" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="J10" t="n">
-        <v>8.0</v>
+        <v>213.0</v>
       </c>
       <c r="K10" t="n">
-        <v>9.0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="11">
@@ -571,34 +589,104 @@
         <v>11</v>
       </c>
       <c r="B11" t="n" s="0">
+        <v>13.0</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>81.0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>55.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n" s="0">
+        <v>11.0</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2.700000047683716</v>
+      </c>
+      <c r="F12" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" t="s">
+        <v>48</v>
+      </c>
+      <c r="I12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J12" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="K12" t="n">
         <v>2.0</v>
       </c>
-      <c r="C11" t="s" s="0">
-        <v>46</v>
-      </c>
-      <c r="D11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" t="n">
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n" s="0">
+        <v>16.0</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" t="n">
         <v>5.0</v>
       </c>
-      <c r="F11" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G11" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" t="s">
-        <v>32</v>
-      </c>
-      <c r="I11" t="s">
-        <v>16</v>
-      </c>
-      <c r="J11" t="n">
-        <v>213.0</v>
-      </c>
-      <c r="K11" t="n">
-        <v>1.5</v>
+      <c r="F13" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" t="s">
+        <v>52</v>
+      </c>
+      <c r="J13" t="n">
+        <v>123.0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>90.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update on reporting to add indicator and months
</commit_message>
<xml_diff>
--- a/temp/excelTestCheckup.xlsx
+++ b/temp/excelTestCheckup.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>posyandu</t>
   </si>
@@ -45,6 +45,45 @@
   </si>
   <si>
     <t>tinggi</t>
+  </si>
+  <si>
+    <t>usia</t>
+  </si>
+  <si>
+    <t>catatan</t>
+  </si>
+  <si>
+    <t>indikasi</t>
+  </si>
+  <si>
+    <t>POSYANDU Anggrek</t>
+  </si>
+  <si>
+    <t>56643907556</t>
+  </si>
+  <si>
+    <t>Junaidi</t>
+  </si>
+  <si>
+    <t>Jl. Gunung Kidul 12</t>
+  </si>
+  <si>
+    <t>Joko</t>
+  </si>
+  <si>
+    <t>2023-05-08</t>
+  </si>
+  <si>
+    <t>sehat</t>
+  </si>
+  <si>
+    <t>2023-06-05</t>
+  </si>
+  <si>
+    <t>tidak sehat</t>
+  </si>
+  <si>
+    <t>2023-07-31</t>
   </si>
 </sst>
 </file>
@@ -89,23 +128,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="9.73046875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="19.03125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="7.70703125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="11.0703125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="8.70703125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="13.3046875" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="7.3359375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="9.99609375" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.15234375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="12.7421875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="18.03125" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="14.17578125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="15.015625" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="5.84765625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="12.7421875" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="6.01171875" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="4.61328125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -142,6 +182,141 @@
       <c r="K1" t="s" s="0">
         <v>10</v>
       </c>
+      <c r="L1" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B2" t="n" s="0">
+        <v>20.0</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>50.20000076293945</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="K2" t="n">
+        <v>52.0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="M2"/>
+      <c r="N2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B3" t="n" s="0">
+        <v>20.0</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>50.20000076293945</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>56.0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="M3"/>
+      <c r="N3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B4" t="n" s="0">
+        <v>20.0</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>50.20000076293945</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" t="n">
+        <v>4.199999809265137</v>
+      </c>
+      <c r="K4" t="n">
+        <v>55.0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="M4"/>
+      <c r="N4" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>